<commit_message>
Fix crop scenario name
</commit_message>
<xml_diff>
--- a/template_v2.xlsx
+++ b/template_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dpollard/projects/comet/COMET-Farm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43A07B49-477A-3A4F-942D-4D8D3F042D22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAE46DDA-7E3C-3146-90C3-01FCD50B4DCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3060" yWindow="460" windowWidth="30540" windowHeight="20540" xr2:uid="{5384504D-6727-334D-8532-C0C118A2956A}"/>
   </bookViews>
@@ -33,6 +33,7 @@
   </externalReferences>
   <definedNames>
     <definedName name="Crops">[1]Units!$A$2:$A$34</definedName>
+    <definedName name="No">yesno!$A$1:$A$4</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -95,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="169">
   <si>
     <t>Yes</t>
   </si>
@@ -599,6 +600,9 @@
   </si>
   <si>
     <t>Current</t>
+  </si>
+  <si>
+    <t>Name</t>
   </si>
 </sst>
 </file>
@@ -732,7 +736,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -756,6 +760,10 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1275,7 +1283,7 @@
   <dimension ref="A1:P46"/>
   <sheetViews>
     <sheetView showFormulas="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1292,7 +1300,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="3" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
@@ -1300,7 +1308,7 @@
       </c>
     </row>
     <row r="2" spans="1:16" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="12" t="s">
         <v>67</v>
       </c>
       <c r="B2" s="7" t="s">
@@ -1308,7 +1316,7 @@
       </c>
     </row>
     <row r="3" spans="1:16" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="12" t="s">
         <v>69</v>
       </c>
       <c r="B3" s="7" t="s">
@@ -1316,7 +1324,7 @@
       </c>
     </row>
     <row r="4" spans="1:16" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="12" t="s">
         <v>68</v>
       </c>
       <c r="B4" s="7" t="s">
@@ -1324,23 +1332,23 @@
       </c>
     </row>
     <row r="5" spans="1:16" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="15" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="15" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="12" t="s">
         <v>70</v>
       </c>
       <c r="B7" s="7" t="s">
@@ -1348,7 +1356,7 @@
       </c>
     </row>
     <row r="8" spans="1:16" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="12" t="s">
         <v>71</v>
       </c>
       <c r="B8" s="7" t="s">
@@ -1356,79 +1364,84 @@
       </c>
     </row>
     <row r="9" spans="1:16" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="12" t="s">
         <v>118</v>
       </c>
       <c r="B9" s="7"/>
     </row>
     <row r="10" spans="1:16" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="12" t="s">
         <v>66</v>
       </c>
       <c r="B10" s="7"/>
     </row>
     <row r="11" spans="1:16" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="12" t="s">
         <v>119</v>
       </c>
       <c r="B11" s="7"/>
     </row>
     <row r="12" spans="1:16" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="12" t="s">
         <v>120</v>
       </c>
       <c r="B12" s="7"/>
+    </row>
+    <row r="13" spans="1:16" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="11" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="14" spans="1:16" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C14" s="7"/>
     </row>
-    <row r="15" spans="1:16" s="12" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="12" t="s">
+    <row r="15" spans="1:16" s="13" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="E15" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="F15" s="12" t="s">
+      <c r="F15" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="G15" s="12" t="s">
+      <c r="G15" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="H15" s="12" t="s">
+      <c r="H15" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="I15" s="12" t="s">
+      <c r="I15" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="J15" s="12" t="s">
+      <c r="J15" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="K15" s="12" t="s">
+      <c r="K15" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="L15" s="12" t="s">
+      <c r="L15" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="M15" s="13" t="s">
+      <c r="M15" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="N15" s="12" t="s">
+      <c r="N15" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="O15" s="13" t="s">
+      <c r="O15" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="P15" s="12" t="s">
+      <c r="P15" s="13" t="s">
         <v>133</v>
       </c>
     </row>
@@ -3389,7 +3402,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update template and script to separate out current practices and scenario practices, plus option for a scenario b
</commit_message>
<xml_diff>
--- a/template_v2.xlsx
+++ b/template_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dpollard/projects/comet/COMET-Farm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAE46DDA-7E3C-3146-90C3-01FCD50B4DCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23469475-2BD2-0740-AAE1-E55CE4EABE42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3060" yWindow="460" windowWidth="30540" windowHeight="20540" xr2:uid="{5384504D-6727-334D-8532-C0C118A2956A}"/>
   </bookViews>
@@ -1283,10 +1283,10 @@
   <dimension ref="A1:P46"/>
   <sheetViews>
     <sheetView showFormulas="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="25" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="4"/>
     <col min="2" max="2" width="9.5" style="4" bestFit="1" customWidth="1"/>
@@ -1367,25 +1367,21 @@
       <c r="A9" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="B9" s="7"/>
     </row>
     <row r="10" spans="1:16" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="B10" s="7"/>
     </row>
     <row r="11" spans="1:16" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="B11" s="7"/>
     </row>
     <row r="12" spans="1:16" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="B12" s="7"/>
     </row>
     <row r="13" spans="1:16" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
@@ -2445,7 +2441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:16" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:16" ht="25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A37" s="4">
         <v>2020</v>
       </c>
@@ -2495,7 +2491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:16" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:16" ht="25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A38" s="4">
         <v>2021</v>
       </c>
@@ -2545,7 +2541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:16" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:16" ht="25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A39" s="4">
         <v>2022</v>
       </c>
@@ -2595,7 +2591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:16" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:16" ht="25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A40" s="4">
         <v>2023</v>
       </c>
@@ -2645,7 +2641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:16" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:16" ht="25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A41" s="4">
         <v>2024</v>
       </c>
@@ -2695,7 +2691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:16" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:16" ht="25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A42" s="4">
         <v>2025</v>
       </c>
@@ -2745,7 +2741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:16" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:16" ht="25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A43" s="4">
         <v>2026</v>
       </c>
@@ -2795,7 +2791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:16" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:16" ht="25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A44" s="4">
         <v>2027</v>
       </c>
@@ -2845,7 +2841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:16" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:16" ht="25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A45" s="4">
         <v>2028</v>
       </c>
@@ -2895,7 +2891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:16" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:16" ht="25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A46" s="4">
         <v>2029</v>
       </c>
@@ -3018,7 +3014,7 @@
           <x14:formula1>
             <xm:f>binary!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>C14 B8:B12</xm:sqref>
+          <xm:sqref>C14 B8</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Match generated XML to exported sample from comet-farm
</commit_message>
<xml_diff>
--- a/template_v2.xlsx
+++ b/template_v2.xlsx
@@ -8,28 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dpollard/projects/comet/COMET-Farm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23469475-2BD2-0740-AAE1-E55CE4EABE42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C5F4F41-57D5-7A4D-AF41-87BC70741FF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3060" yWindow="460" windowWidth="30540" windowHeight="20540" xr2:uid="{5384504D-6727-334D-8532-C0C118A2956A}"/>
+    <workbookView xWindow="0" yWindow="480" windowWidth="32720" windowHeight="20540" xr2:uid="{5384504D-6727-334D-8532-C0C118A2956A}"/>
   </bookViews>
   <sheets>
     <sheet name="scenario" sheetId="1" r:id="rId1"/>
-    <sheet name="eep" sheetId="13" r:id="rId2"/>
-    <sheet name="pre1980" sheetId="6" r:id="rId3"/>
-    <sheet name="yr80" sheetId="7" r:id="rId4"/>
-    <sheet name="yesno" sheetId="2" r:id="rId5"/>
-    <sheet name="crops" sheetId="3" r:id="rId6"/>
-    <sheet name="covercrops" sheetId="4" r:id="rId7"/>
-    <sheet name="treesvines" sheetId="5" r:id="rId8"/>
-    <sheet name="binary" sheetId="9" r:id="rId9"/>
-    <sheet name="tillagetype" sheetId="10" r:id="rId10"/>
-    <sheet name="napplicationtype" sheetId="11" r:id="rId11"/>
-    <sheet name="napplicationmethod" sheetId="12" r:id="rId12"/>
-    <sheet name="tillage" sheetId="8" r:id="rId13"/>
-    <sheet name="CRP" sheetId="14" r:id="rId14"/>
+    <sheet name="YN" sheetId="15" r:id="rId2"/>
+    <sheet name="eep" sheetId="13" r:id="rId3"/>
+    <sheet name="pre1980" sheetId="6" r:id="rId4"/>
+    <sheet name="yr80" sheetId="7" r:id="rId5"/>
+    <sheet name="yesno" sheetId="2" r:id="rId6"/>
+    <sheet name="crops" sheetId="3" r:id="rId7"/>
+    <sheet name="covercrops" sheetId="4" r:id="rId8"/>
+    <sheet name="treesvines" sheetId="5" r:id="rId9"/>
+    <sheet name="TF" sheetId="16" r:id="rId10"/>
+    <sheet name="binary" sheetId="9" r:id="rId11"/>
+    <sheet name="tillagetype" sheetId="10" r:id="rId12"/>
+    <sheet name="napplicationtype" sheetId="11" r:id="rId13"/>
+    <sheet name="napplicationmethod" sheetId="12" r:id="rId14"/>
+    <sheet name="tillage" sheetId="8" r:id="rId15"/>
+    <sheet name="CRP" sheetId="14" r:id="rId16"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId15"/>
+    <externalReference r:id="rId17"/>
   </externalReferences>
   <definedNames>
     <definedName name="Crops">[1]Units!$A$2:$A$34</definedName>
@@ -96,7 +98,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="171">
   <si>
     <t>Yes</t>
   </si>
@@ -603,6 +605,12 @@
   </si>
   <si>
     <t>Name</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
@@ -1280,10 +1288,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B479D4AE-FA7D-CA44-BF82-B5408D6E0BCF}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:P46"/>
+  <dimension ref="A1:P57"/>
   <sheetViews>
-    <sheetView showFormulas="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView showFormulas="1" tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48:D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="25" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -1452,7 +1460,7 @@
         <v>137</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>1</v>
+        <v>169</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>137</v>
@@ -1460,7 +1468,7 @@
       <c r="F16" s="7">
         <v>100</v>
       </c>
-      <c r="G16" s="10" t="s">
+      <c r="G16" s="10" t="b">
         <v>1</v>
       </c>
       <c r="H16" s="7">
@@ -1502,7 +1510,7 @@
         <v>138</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>1</v>
+        <v>169</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>138</v>
@@ -1510,7 +1518,7 @@
       <c r="F17" s="7">
         <v>100</v>
       </c>
-      <c r="G17" s="10" t="s">
+      <c r="G17" s="10" t="b">
         <v>1</v>
       </c>
       <c r="H17" s="7">
@@ -1552,7 +1560,7 @@
         <v>139</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>1</v>
+        <v>169</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>139</v>
@@ -1560,7 +1568,7 @@
       <c r="F18" s="7">
         <v>100</v>
       </c>
-      <c r="G18" s="10" t="s">
+      <c r="G18" s="10" t="b">
         <v>1</v>
       </c>
       <c r="H18" s="7">
@@ -1602,7 +1610,7 @@
         <v>140</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>1</v>
+        <v>169</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>140</v>
@@ -1610,7 +1618,7 @@
       <c r="F19" s="7">
         <v>100</v>
       </c>
-      <c r="G19" s="10" t="s">
+      <c r="G19" s="10" t="b">
         <v>1</v>
       </c>
       <c r="H19" s="7">
@@ -1652,7 +1660,7 @@
         <v>141</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>1</v>
+        <v>169</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>141</v>
@@ -1660,7 +1668,7 @@
       <c r="F20" s="7">
         <v>100</v>
       </c>
-      <c r="G20" s="10" t="s">
+      <c r="G20" s="10" t="b">
         <v>1</v>
       </c>
       <c r="H20" s="7">
@@ -1702,7 +1710,7 @@
         <v>142</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>1</v>
+        <v>169</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>142</v>
@@ -1710,7 +1718,7 @@
       <c r="F21" s="7">
         <v>100</v>
       </c>
-      <c r="G21" s="10" t="s">
+      <c r="G21" s="10" t="b">
         <v>1</v>
       </c>
       <c r="H21" s="7">
@@ -1752,7 +1760,7 @@
         <v>143</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>1</v>
+        <v>169</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>143</v>
@@ -1760,7 +1768,7 @@
       <c r="F22" s="7">
         <v>100</v>
       </c>
-      <c r="G22" s="10" t="s">
+      <c r="G22" s="10" t="b">
         <v>1</v>
       </c>
       <c r="H22" s="7">
@@ -1802,7 +1810,7 @@
         <v>144</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>1</v>
+        <v>169</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>144</v>
@@ -1810,7 +1818,7 @@
       <c r="F23" s="7">
         <v>100</v>
       </c>
-      <c r="G23" s="10" t="s">
+      <c r="G23" s="10" t="b">
         <v>1</v>
       </c>
       <c r="H23" s="7">
@@ -1852,7 +1860,7 @@
         <v>145</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>1</v>
+        <v>169</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>145</v>
@@ -1860,7 +1868,7 @@
       <c r="F24" s="7">
         <v>100</v>
       </c>
-      <c r="G24" s="10" t="s">
+      <c r="G24" s="10" t="b">
         <v>1</v>
       </c>
       <c r="H24" s="7">
@@ -1902,7 +1910,7 @@
         <v>146</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>1</v>
+        <v>169</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>146</v>
@@ -1910,7 +1918,7 @@
       <c r="F25" s="7">
         <v>100</v>
       </c>
-      <c r="G25" s="10" t="s">
+      <c r="G25" s="10" t="b">
         <v>1</v>
       </c>
       <c r="H25" s="7">
@@ -1952,7 +1960,7 @@
         <v>147</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>1</v>
+        <v>169</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>147</v>
@@ -1960,7 +1968,7 @@
       <c r="F26" s="7">
         <v>100</v>
       </c>
-      <c r="G26" s="10" t="s">
+      <c r="G26" s="10" t="b">
         <v>1</v>
       </c>
       <c r="H26" s="7">
@@ -2002,7 +2010,7 @@
         <v>148</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>1</v>
+        <v>169</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>148</v>
@@ -2010,7 +2018,7 @@
       <c r="F27" s="7">
         <v>100</v>
       </c>
-      <c r="G27" s="10" t="s">
+      <c r="G27" s="10" t="b">
         <v>1</v>
       </c>
       <c r="H27" s="7">
@@ -2052,7 +2060,7 @@
         <v>149</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>1</v>
+        <v>169</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>149</v>
@@ -2060,7 +2068,7 @@
       <c r="F28" s="7">
         <v>100</v>
       </c>
-      <c r="G28" s="10" t="s">
+      <c r="G28" s="10" t="b">
         <v>1</v>
       </c>
       <c r="H28" s="7">
@@ -2102,7 +2110,7 @@
         <v>150</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>1</v>
+        <v>169</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>150</v>
@@ -2110,7 +2118,7 @@
       <c r="F29" s="7">
         <v>100</v>
       </c>
-      <c r="G29" s="10" t="s">
+      <c r="G29" s="10" t="b">
         <v>1</v>
       </c>
       <c r="H29" s="7">
@@ -2152,7 +2160,7 @@
         <v>151</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>1</v>
+        <v>169</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>151</v>
@@ -2160,7 +2168,7 @@
       <c r="F30" s="7">
         <v>100</v>
       </c>
-      <c r="G30" s="10" t="s">
+      <c r="G30" s="10" t="b">
         <v>1</v>
       </c>
       <c r="H30" s="7">
@@ -2202,7 +2210,7 @@
         <v>152</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>1</v>
+        <v>169</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>152</v>
@@ -2210,7 +2218,7 @@
       <c r="F31" s="7">
         <v>100</v>
       </c>
-      <c r="G31" s="10" t="s">
+      <c r="G31" s="10" t="b">
         <v>1</v>
       </c>
       <c r="H31" s="7">
@@ -2252,7 +2260,7 @@
         <v>153</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>1</v>
+        <v>169</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>153</v>
@@ -2260,7 +2268,7 @@
       <c r="F32" s="7">
         <v>100</v>
       </c>
-      <c r="G32" s="10" t="s">
+      <c r="G32" s="10" t="b">
         <v>1</v>
       </c>
       <c r="H32" s="7">
@@ -2302,7 +2310,7 @@
         <v>154</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>1</v>
+        <v>169</v>
       </c>
       <c r="E33" s="7" t="s">
         <v>154</v>
@@ -2310,7 +2318,7 @@
       <c r="F33" s="7">
         <v>100</v>
       </c>
-      <c r="G33" s="10" t="s">
+      <c r="G33" s="10" t="b">
         <v>1</v>
       </c>
       <c r="H33" s="7">
@@ -2352,7 +2360,7 @@
         <v>155</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>1</v>
+        <v>169</v>
       </c>
       <c r="E34" s="7" t="s">
         <v>155</v>
@@ -2360,7 +2368,7 @@
       <c r="F34" s="7">
         <v>100</v>
       </c>
-      <c r="G34" s="10" t="s">
+      <c r="G34" s="10" t="b">
         <v>1</v>
       </c>
       <c r="H34" s="7">
@@ -2402,7 +2410,7 @@
         <v>156</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>1</v>
+        <v>169</v>
       </c>
       <c r="E35" s="7" t="s">
         <v>156</v>
@@ -2410,7 +2418,7 @@
       <c r="F35" s="7">
         <v>100</v>
       </c>
-      <c r="G35" s="10" t="s">
+      <c r="G35" s="10" t="b">
         <v>1</v>
       </c>
       <c r="H35" s="7">
@@ -2452,7 +2460,7 @@
         <v>157</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>1</v>
+        <v>169</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>157</v>
@@ -2460,7 +2468,7 @@
       <c r="F37" s="7">
         <v>100</v>
       </c>
-      <c r="G37" s="10" t="s">
+      <c r="G37" s="10" t="b">
         <v>1</v>
       </c>
       <c r="H37" s="7">
@@ -2502,7 +2510,7 @@
         <v>158</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>1</v>
+        <v>169</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>158</v>
@@ -2510,7 +2518,7 @@
       <c r="F38" s="7">
         <v>100</v>
       </c>
-      <c r="G38" s="10" t="s">
+      <c r="G38" s="10" t="b">
         <v>1</v>
       </c>
       <c r="H38" s="7">
@@ -2552,7 +2560,7 @@
         <v>159</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>1</v>
+        <v>169</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>159</v>
@@ -2560,7 +2568,7 @@
       <c r="F39" s="7">
         <v>100</v>
       </c>
-      <c r="G39" s="10" t="s">
+      <c r="G39" s="10" t="b">
         <v>1</v>
       </c>
       <c r="H39" s="7">
@@ -2602,7 +2610,7 @@
         <v>160</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>1</v>
+        <v>169</v>
       </c>
       <c r="E40" s="4" t="s">
         <v>160</v>
@@ -2610,7 +2618,7 @@
       <c r="F40" s="7">
         <v>100</v>
       </c>
-      <c r="G40" s="10" t="s">
+      <c r="G40" s="10" t="b">
         <v>1</v>
       </c>
       <c r="H40" s="7">
@@ -2652,7 +2660,7 @@
         <v>161</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>1</v>
+        <v>169</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>161</v>
@@ -2660,7 +2668,7 @@
       <c r="F41" s="7">
         <v>100</v>
       </c>
-      <c r="G41" s="10" t="s">
+      <c r="G41" s="10" t="b">
         <v>1</v>
       </c>
       <c r="H41" s="7">
@@ -2702,7 +2710,7 @@
         <v>162</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>1</v>
+        <v>169</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>162</v>
@@ -2710,7 +2718,7 @@
       <c r="F42" s="7">
         <v>100</v>
       </c>
-      <c r="G42" s="10" t="s">
+      <c r="G42" s="10" t="b">
         <v>1</v>
       </c>
       <c r="H42" s="7">
@@ -2752,7 +2760,7 @@
         <v>163</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>1</v>
+        <v>169</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>163</v>
@@ -2760,7 +2768,7 @@
       <c r="F43" s="7">
         <v>100</v>
       </c>
-      <c r="G43" s="10" t="s">
+      <c r="G43" s="10" t="b">
         <v>1</v>
       </c>
       <c r="H43" s="7">
@@ -2802,7 +2810,7 @@
         <v>164</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>1</v>
+        <v>169</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>164</v>
@@ -2810,7 +2818,7 @@
       <c r="F44" s="7">
         <v>100</v>
       </c>
-      <c r="G44" s="10" t="s">
+      <c r="G44" s="10" t="b">
         <v>1</v>
       </c>
       <c r="H44" s="7">
@@ -2852,7 +2860,7 @@
         <v>165</v>
       </c>
       <c r="D45" s="10" t="s">
-        <v>1</v>
+        <v>169</v>
       </c>
       <c r="E45" s="4" t="s">
         <v>165</v>
@@ -2860,7 +2868,7 @@
       <c r="F45" s="7">
         <v>100</v>
       </c>
-      <c r="G45" s="10" t="s">
+      <c r="G45" s="10" t="b">
         <v>1</v>
       </c>
       <c r="H45" s="7">
@@ -2902,7 +2910,7 @@
         <v>166</v>
       </c>
       <c r="D46" s="10" t="s">
-        <v>1</v>
+        <v>169</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>166</v>
@@ -2910,7 +2918,7 @@
       <c r="F46" s="7">
         <v>100</v>
       </c>
-      <c r="G46" s="10" t="s">
+      <c r="G46" s="10" t="b">
         <v>1</v>
       </c>
       <c r="H46" s="7">
@@ -2938,6 +2946,476 @@
         <v>123</v>
       </c>
       <c r="P46" s="10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" ht="25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="4">
+        <v>2020</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="F48" s="7">
+        <v>100</v>
+      </c>
+      <c r="G48" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="H48" s="7">
+        <v>0</v>
+      </c>
+      <c r="I48" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="J48" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="K48" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="L48" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="M48" s="7">
+        <v>100</v>
+      </c>
+      <c r="N48" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="O48" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="P48" s="10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" ht="25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="4">
+        <v>2021</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="D49" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="F49" s="7">
+        <v>100</v>
+      </c>
+      <c r="G49" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="H49" s="7">
+        <v>0</v>
+      </c>
+      <c r="I49" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="J49" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="K49" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="L49" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="M49" s="7">
+        <v>100</v>
+      </c>
+      <c r="N49" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="O49" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="P49" s="10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" ht="25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="4">
+        <v>2022</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="D50" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="F50" s="7">
+        <v>100</v>
+      </c>
+      <c r="G50" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="H50" s="7">
+        <v>0</v>
+      </c>
+      <c r="I50" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="J50" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="K50" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="L50" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="M50" s="7">
+        <v>100</v>
+      </c>
+      <c r="N50" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="O50" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="P50" s="10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" ht="25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="4">
+        <v>2023</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="D51" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="F51" s="7">
+        <v>100</v>
+      </c>
+      <c r="G51" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="H51" s="7">
+        <v>0</v>
+      </c>
+      <c r="I51" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="J51" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="K51" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="L51" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="M51" s="7">
+        <v>100</v>
+      </c>
+      <c r="N51" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="O51" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="P51" s="10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" ht="25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="4">
+        <v>2024</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="F52" s="7">
+        <v>100</v>
+      </c>
+      <c r="G52" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="H52" s="7">
+        <v>0</v>
+      </c>
+      <c r="I52" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="J52" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="K52" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="L52" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="M52" s="7">
+        <v>100</v>
+      </c>
+      <c r="N52" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="O52" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="P52" s="10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" ht="25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="4">
+        <v>2025</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="D53" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="F53" s="7">
+        <v>100</v>
+      </c>
+      <c r="G53" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="H53" s="7">
+        <v>0</v>
+      </c>
+      <c r="I53" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="J53" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="K53" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="L53" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="M53" s="7">
+        <v>100</v>
+      </c>
+      <c r="N53" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="O53" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="P53" s="10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" ht="25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="4">
+        <v>2026</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="D54" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="F54" s="7">
+        <v>100</v>
+      </c>
+      <c r="G54" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="H54" s="7">
+        <v>0</v>
+      </c>
+      <c r="I54" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="J54" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="K54" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="L54" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="M54" s="7">
+        <v>100</v>
+      </c>
+      <c r="N54" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="O54" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="P54" s="10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" ht="25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="4">
+        <v>2027</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="D55" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="F55" s="7">
+        <v>100</v>
+      </c>
+      <c r="G55" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="H55" s="7">
+        <v>0</v>
+      </c>
+      <c r="I55" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="J55" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="K55" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="L55" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="M55" s="7">
+        <v>100</v>
+      </c>
+      <c r="N55" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="O55" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="P55" s="10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" ht="25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="4">
+        <v>2028</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D56" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="F56" s="7">
+        <v>100</v>
+      </c>
+      <c r="G56" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="H56" s="7">
+        <v>0</v>
+      </c>
+      <c r="I56" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="J56" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="K56" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="L56" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="M56" s="7">
+        <v>100</v>
+      </c>
+      <c r="N56" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="O56" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="P56" s="10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" ht="25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="4">
+        <v>2029</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="D57" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="F57" s="7">
+        <v>100</v>
+      </c>
+      <c r="G57" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="H57" s="7">
+        <v>0</v>
+      </c>
+      <c r="I57" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="J57" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="K57" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="L57" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="M57" s="7">
+        <v>100</v>
+      </c>
+      <c r="N57" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="O57" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="P57" s="10" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2949,18 +3427,18 @@
   <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="11">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="13">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Choose" prompt="Make a choice" xr:uid="{C3AD2C11-A234-5E47-8591-D75A01B1DC7E}">
           <x14:formula1>
             <xm:f>yesno!$A$1:$A$2</xm:f>
           </x14:formula1>
-          <xm:sqref>D16:D35 G37:H46 B5 D37:D46 G16:H35 P16:P35 P37:P46</xm:sqref>
+          <xm:sqref>H48:H57 H16:H35 B5 H37:H46 P48:P57 P16:P35 P37:P46</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Choose a crop" error="Choose a crop" promptTitle="Crop" prompt="choose crop" xr:uid="{97E5F41B-79F3-664A-BF6C-E828031A2348}">
           <x14:formula1>
             <xm:f>crops!$A$2:$A$34</xm:f>
           </x14:formula1>
-          <xm:sqref>B37:B46 B16:B35</xm:sqref>
+          <xm:sqref>B37:B46 B16:B35 B48:B57</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C662B32F-7BC6-3241-AB1A-835972BD7A98}">
           <x14:formula1>
@@ -2984,25 +3462,25 @@
           <x14:formula1>
             <xm:f>tillagetype!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>I16:I35 I37:I46</xm:sqref>
+          <xm:sqref>I16:I35 I37:I46 I48:I57</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{62EC0EF5-D38F-C34F-A670-E8811702E4E5}">
           <x14:formula1>
             <xm:f>napplicationtype!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>K16:K35 K37:K46</xm:sqref>
+          <xm:sqref>K16:K35 K37:K46 K48:K57</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4B3F0D01-0C61-A842-820D-08C228960E92}">
           <x14:formula1>
             <xm:f>napplicationmethod!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>O16:O35 O37:O46</xm:sqref>
+          <xm:sqref>O16:O35 O37:O46 O48:O57</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{99E16EBF-9E61-1645-BD5E-612799654BF7}">
           <x14:formula1>
             <xm:f>eep!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>N16:N35 N37:N46</xm:sqref>
+          <xm:sqref>N16:N35 N37:N46 N48:N57</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Choose" prompt="Make a choice" xr:uid="{06A2A93F-3AE0-7547-A6B8-80C32B43ECDC}">
           <x14:formula1>
@@ -3016,6 +3494,18 @@
           </x14:formula1>
           <xm:sqref>C14 B8</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Choose" prompt="Make a choice" xr:uid="{8F48DC1A-6F30-9F4D-AF45-BC62A834EB1F}">
+          <x14:formula1>
+            <xm:f>TF!$A$1:$A$2</xm:f>
+          </x14:formula1>
+          <xm:sqref>G16:G35 G37:G46 G48:G57</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Choose" prompt="Make a choice" xr:uid="{E7666449-C24D-574C-B125-F28CC372BDB7}">
+          <x14:formula1>
+            <xm:f>YN!$A$1:$A$2</xm:f>
+          </x14:formula1>
+          <xm:sqref>D16:D35 D37:D46 D48:D57</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -3023,6 +3513,57 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29EA7B87-79B2-534A-945E-D61302BCD4A9}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8DD3F6A-7E39-6C4F-A01B-DC7DE0459EB8}">
+  <sheetPr codeName="Sheet9"/>
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8E3703A-3DA3-1343-819D-167B46A84488}">
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:A10"/>
@@ -3091,7 +3632,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D564B03-164D-154C-8A71-3191222F40FA}">
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:A9"/>
@@ -3156,7 +3697,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F3C9515-4904-A94F-84AB-7579174EE5B8}">
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:A5"/>
@@ -3197,7 +3738,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D6820C7-4691-BF4C-99FC-BAF63356F37A}">
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:A3"/>
@@ -3231,7 +3772,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE56A43D-C66D-794A-B955-261E54B68E02}">
   <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:A3"/>
@@ -3263,13 +3804,36 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4844B9D2-9681-884A-A06D-234A743A182D}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A1:A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB5D2F5-09C0-5D41-B791-F567343A980B}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -3293,7 +3857,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29BF609B-1F57-E245-805C-345CE448249A}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:A4"/>
@@ -3331,7 +3895,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1425D712-AC41-924C-A9AE-3E51B7EDF505}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:A9"/>
@@ -3392,7 +3956,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3DA19AE-C34D-9342-969B-07301959E3E1}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:A3"/>
@@ -3423,7 +3987,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A963F5CA-9031-6442-8BE3-8F7DE6802028}">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:B34"/>
@@ -3714,7 +4278,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DF27384-76BF-B542-A9B2-05B92B0EBBB8}">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:B14"/>
@@ -3845,7 +4409,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF5DA86C-720F-E54A-B3B0-93F1CA124C2E}">
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:B14"/>
@@ -3935,30 +4499,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8DD3F6A-7E39-6C4F-A01B-DC7DE0459EB8}">
-  <sheetPr codeName="Sheet9"/>
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Finally figured out what was wrong!!!! Knew it would be something stupid and it was... -> missing </Project>
</commit_message>
<xml_diff>
--- a/template_v2.xlsx
+++ b/template_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dpollard/projects/comet/COMET-Farm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C5F4F41-57D5-7A4D-AF41-87BC70741FF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC72EA96-E374-4145-9C35-5BF235217FB1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="480" windowWidth="32720" windowHeight="20540" xr2:uid="{5384504D-6727-334D-8532-C0C118A2956A}"/>
   </bookViews>
@@ -98,7 +98,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="261">
   <si>
     <t>Yes</t>
   </si>
@@ -601,9 +601,6 @@
     <t>"01/01/2029"</t>
   </si>
   <si>
-    <t>Current</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -611,6 +608,279 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>"10/01/2000"</t>
+  </si>
+  <si>
+    <t>"10/01/2001"</t>
+  </si>
+  <si>
+    <t>"10/01/2002"</t>
+  </si>
+  <si>
+    <t>"10/01/2003"</t>
+  </si>
+  <si>
+    <t>"10/01/2004"</t>
+  </si>
+  <si>
+    <t>"10/01/2005"</t>
+  </si>
+  <si>
+    <t>"10/01/2008"</t>
+  </si>
+  <si>
+    <t>"10/01/2007"</t>
+  </si>
+  <si>
+    <t>"10/01/2006"</t>
+  </si>
+  <si>
+    <t>"10/01/2009"</t>
+  </si>
+  <si>
+    <t>"10/01/2010"</t>
+  </si>
+  <si>
+    <t>"10/01/2011"</t>
+  </si>
+  <si>
+    <t>"10/01/2012"</t>
+  </si>
+  <si>
+    <t>"10/01/2013"</t>
+  </si>
+  <si>
+    <t>"10/01/2014"</t>
+  </si>
+  <si>
+    <t>"10/01/2015"</t>
+  </si>
+  <si>
+    <t>"10/01/2016"</t>
+  </si>
+  <si>
+    <t>"10/01/2017"</t>
+  </si>
+  <si>
+    <t>"10/01/2018"</t>
+  </si>
+  <si>
+    <t>"10/01/2019"</t>
+  </si>
+  <si>
+    <t>"10/01/2020"</t>
+  </si>
+  <si>
+    <t>"10/01/2021"</t>
+  </si>
+  <si>
+    <t>"10/01/2022"</t>
+  </si>
+  <si>
+    <t>"10/01/2023"</t>
+  </si>
+  <si>
+    <t>"10/01/2024"</t>
+  </si>
+  <si>
+    <t>"10/01/2025"</t>
+  </si>
+  <si>
+    <t>"10/01/2026"</t>
+  </si>
+  <si>
+    <t>"10/01/2027"</t>
+  </si>
+  <si>
+    <t>"10/01/2028"</t>
+  </si>
+  <si>
+    <t>"10/01/2029"</t>
+  </si>
+  <si>
+    <t>"05/01/2000"</t>
+  </si>
+  <si>
+    <t>"05/01/2001"</t>
+  </si>
+  <si>
+    <t>"05/01/2002"</t>
+  </si>
+  <si>
+    <t>"05/01/2003"</t>
+  </si>
+  <si>
+    <t>"05/01/2004"</t>
+  </si>
+  <si>
+    <t>"05/01/2005"</t>
+  </si>
+  <si>
+    <t>"05/01/2006"</t>
+  </si>
+  <si>
+    <t>"05/01/2007"</t>
+  </si>
+  <si>
+    <t>"05/01/2008"</t>
+  </si>
+  <si>
+    <t>"05/01/2009"</t>
+  </si>
+  <si>
+    <t>"05/01/2010"</t>
+  </si>
+  <si>
+    <t>"05/01/2011"</t>
+  </si>
+  <si>
+    <t>"05/01/2012"</t>
+  </si>
+  <si>
+    <t>"05/01/2013"</t>
+  </si>
+  <si>
+    <t>"05/01/2014"</t>
+  </si>
+  <si>
+    <t>"05/01/2015"</t>
+  </si>
+  <si>
+    <t>"05/01/2016"</t>
+  </si>
+  <si>
+    <t>"05/01/2017"</t>
+  </si>
+  <si>
+    <t>"05/01/2018"</t>
+  </si>
+  <si>
+    <t>"05/01/2019"</t>
+  </si>
+  <si>
+    <t>"05/01/2021"</t>
+  </si>
+  <si>
+    <t>"05/01/2020"</t>
+  </si>
+  <si>
+    <t>"05/01/2022"</t>
+  </si>
+  <si>
+    <t>"05/01/2023"</t>
+  </si>
+  <si>
+    <t>"05/01/2024"</t>
+  </si>
+  <si>
+    <t>"05/01/2025"</t>
+  </si>
+  <si>
+    <t>"05/01/2026"</t>
+  </si>
+  <si>
+    <t>"05/01/2027"</t>
+  </si>
+  <si>
+    <t>"05/01/2028"</t>
+  </si>
+  <si>
+    <t>"05/01/2029"</t>
+  </si>
+  <si>
+    <t>no till</t>
+  </si>
+  <si>
+    <t>"05/09/2000"</t>
+  </si>
+  <si>
+    <t>"05/09/2001"</t>
+  </si>
+  <si>
+    <t>"05/09/2002"</t>
+  </si>
+  <si>
+    <t>"05/09/2003"</t>
+  </si>
+  <si>
+    <t>"05/09/2004"</t>
+  </si>
+  <si>
+    <t>"05/09/2005"</t>
+  </si>
+  <si>
+    <t>"05/09/2006"</t>
+  </si>
+  <si>
+    <t>"05/09/2007"</t>
+  </si>
+  <si>
+    <t>"05/09/2008"</t>
+  </si>
+  <si>
+    <t>"05/09/2009"</t>
+  </si>
+  <si>
+    <t>"05/09/2010"</t>
+  </si>
+  <si>
+    <t>"05/09/2011"</t>
+  </si>
+  <si>
+    <t>"05/09/2012"</t>
+  </si>
+  <si>
+    <t>"05/09/2013"</t>
+  </si>
+  <si>
+    <t>"05/09/2014"</t>
+  </si>
+  <si>
+    <t>"05/09/2015"</t>
+  </si>
+  <si>
+    <t>"05/09/2016"</t>
+  </si>
+  <si>
+    <t>"05/09/2017"</t>
+  </si>
+  <si>
+    <t>"05/09/2018"</t>
+  </si>
+  <si>
+    <t>"05/09/2019"</t>
+  </si>
+  <si>
+    <t>"05/09/2020"</t>
+  </si>
+  <si>
+    <t>"05/09/2021"</t>
+  </si>
+  <si>
+    <t>"05/09/2022"</t>
+  </si>
+  <si>
+    <t>"05/09/2023"</t>
+  </si>
+  <si>
+    <t>"05/09/2024"</t>
+  </si>
+  <si>
+    <t>"05/09/2025"</t>
+  </si>
+  <si>
+    <t>"05/09/2026"</t>
+  </si>
+  <si>
+    <t>"05/09/2027"</t>
+  </si>
+  <si>
+    <t>"05/09/2028"</t>
+  </si>
+  <si>
+    <t>"05/09/2029"</t>
   </si>
 </sst>
 </file>
@@ -1290,8 +1560,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:P57"/>
   <sheetViews>
-    <sheetView showFormulas="1" tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48:D57"/>
+    <sheetView showFormulas="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M50" sqref="M50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="25" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -1360,7 +1630,7 @@
         <v>70</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>167</v>
+        <v>230</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1393,7 +1663,7 @@
     </row>
     <row r="13" spans="1:16" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1460,10 +1730,10 @@
         <v>137</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>137</v>
+        <v>170</v>
       </c>
       <c r="F16" s="7">
         <v>100</v>
@@ -1478,13 +1748,13 @@
         <v>97</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>137</v>
+        <v>200</v>
       </c>
       <c r="K16" s="7" t="s">
         <v>109</v>
       </c>
       <c r="L16" s="7" t="s">
-        <v>137</v>
+        <v>231</v>
       </c>
       <c r="M16" s="7">
         <v>100</v>
@@ -1510,10 +1780,10 @@
         <v>138</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>138</v>
+        <v>171</v>
       </c>
       <c r="F17" s="7">
         <v>100</v>
@@ -1528,13 +1798,13 @@
         <v>97</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>138</v>
+        <v>201</v>
       </c>
       <c r="K17" s="7" t="s">
         <v>109</v>
       </c>
       <c r="L17" s="7" t="s">
-        <v>138</v>
+        <v>232</v>
       </c>
       <c r="M17" s="7">
         <v>100</v>
@@ -1560,10 +1830,10 @@
         <v>139</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>139</v>
+        <v>172</v>
       </c>
       <c r="F18" s="7">
         <v>100</v>
@@ -1578,13 +1848,13 @@
         <v>97</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>139</v>
+        <v>202</v>
       </c>
       <c r="K18" s="7" t="s">
         <v>109</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>139</v>
+        <v>233</v>
       </c>
       <c r="M18" s="7">
         <v>100</v>
@@ -1610,10 +1880,10 @@
         <v>140</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>140</v>
+        <v>173</v>
       </c>
       <c r="F19" s="7">
         <v>100</v>
@@ -1628,13 +1898,13 @@
         <v>97</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>140</v>
+        <v>203</v>
       </c>
       <c r="K19" s="7" t="s">
         <v>109</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>140</v>
+        <v>234</v>
       </c>
       <c r="M19" s="7">
         <v>100</v>
@@ -1660,10 +1930,10 @@
         <v>141</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>141</v>
+        <v>174</v>
       </c>
       <c r="F20" s="7">
         <v>100</v>
@@ -1678,13 +1948,13 @@
         <v>97</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>141</v>
+        <v>204</v>
       </c>
       <c r="K20" s="7" t="s">
         <v>109</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>141</v>
+        <v>235</v>
       </c>
       <c r="M20" s="7">
         <v>100</v>
@@ -1710,10 +1980,10 @@
         <v>142</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>142</v>
+        <v>175</v>
       </c>
       <c r="F21" s="7">
         <v>100</v>
@@ -1728,13 +1998,13 @@
         <v>97</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>142</v>
+        <v>205</v>
       </c>
       <c r="K21" s="7" t="s">
         <v>109</v>
       </c>
       <c r="L21" s="4" t="s">
-        <v>142</v>
+        <v>236</v>
       </c>
       <c r="M21" s="7">
         <v>100</v>
@@ -1760,10 +2030,10 @@
         <v>143</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>143</v>
+        <v>178</v>
       </c>
       <c r="F22" s="7">
         <v>100</v>
@@ -1778,13 +2048,13 @@
         <v>97</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>143</v>
+        <v>206</v>
       </c>
       <c r="K22" s="7" t="s">
         <v>109</v>
       </c>
       <c r="L22" s="4" t="s">
-        <v>143</v>
+        <v>237</v>
       </c>
       <c r="M22" s="7">
         <v>100</v>
@@ -1810,10 +2080,10 @@
         <v>144</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>144</v>
+        <v>177</v>
       </c>
       <c r="F23" s="7">
         <v>100</v>
@@ -1828,13 +2098,13 @@
         <v>97</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>144</v>
+        <v>207</v>
       </c>
       <c r="K23" s="7" t="s">
         <v>109</v>
       </c>
       <c r="L23" s="4" t="s">
-        <v>144</v>
+        <v>238</v>
       </c>
       <c r="M23" s="7">
         <v>100</v>
@@ -1860,10 +2130,10 @@
         <v>145</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>145</v>
+        <v>176</v>
       </c>
       <c r="F24" s="7">
         <v>100</v>
@@ -1878,13 +2148,13 @@
         <v>97</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>145</v>
+        <v>208</v>
       </c>
       <c r="K24" s="7" t="s">
         <v>109</v>
       </c>
       <c r="L24" s="4" t="s">
-        <v>145</v>
+        <v>239</v>
       </c>
       <c r="M24" s="7">
         <v>100</v>
@@ -1910,10 +2180,10 @@
         <v>146</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>146</v>
+        <v>179</v>
       </c>
       <c r="F25" s="7">
         <v>100</v>
@@ -1928,13 +2198,13 @@
         <v>97</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>146</v>
+        <v>209</v>
       </c>
       <c r="K25" s="7" t="s">
         <v>109</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>146</v>
+        <v>240</v>
       </c>
       <c r="M25" s="7">
         <v>100</v>
@@ -1960,10 +2230,10 @@
         <v>147</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>147</v>
+        <v>180</v>
       </c>
       <c r="F26" s="7">
         <v>100</v>
@@ -1978,13 +2248,13 @@
         <v>97</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>147</v>
+        <v>210</v>
       </c>
       <c r="K26" s="7" t="s">
         <v>109</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>147</v>
+        <v>241</v>
       </c>
       <c r="M26" s="7">
         <v>100</v>
@@ -2010,10 +2280,10 @@
         <v>148</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>148</v>
+        <v>181</v>
       </c>
       <c r="F27" s="7">
         <v>100</v>
@@ -2028,13 +2298,13 @@
         <v>97</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>148</v>
+        <v>211</v>
       </c>
       <c r="K27" s="7" t="s">
         <v>109</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>148</v>
+        <v>242</v>
       </c>
       <c r="M27" s="7">
         <v>100</v>
@@ -2060,10 +2330,10 @@
         <v>149</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>149</v>
+        <v>182</v>
       </c>
       <c r="F28" s="7">
         <v>100</v>
@@ -2078,13 +2348,13 @@
         <v>97</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>149</v>
+        <v>212</v>
       </c>
       <c r="K28" s="7" t="s">
         <v>109</v>
       </c>
       <c r="L28" s="4" t="s">
-        <v>149</v>
+        <v>243</v>
       </c>
       <c r="M28" s="7">
         <v>100</v>
@@ -2110,10 +2380,10 @@
         <v>150</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>150</v>
+        <v>183</v>
       </c>
       <c r="F29" s="7">
         <v>100</v>
@@ -2128,13 +2398,13 @@
         <v>97</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>150</v>
+        <v>213</v>
       </c>
       <c r="K29" s="7" t="s">
         <v>109</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>150</v>
+        <v>244</v>
       </c>
       <c r="M29" s="7">
         <v>100</v>
@@ -2160,10 +2430,10 @@
         <v>151</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>151</v>
+        <v>184</v>
       </c>
       <c r="F30" s="7">
         <v>100</v>
@@ -2178,13 +2448,13 @@
         <v>97</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>151</v>
+        <v>214</v>
       </c>
       <c r="K30" s="7" t="s">
         <v>109</v>
       </c>
       <c r="L30" s="4" t="s">
-        <v>151</v>
+        <v>245</v>
       </c>
       <c r="M30" s="7">
         <v>100</v>
@@ -2210,10 +2480,10 @@
         <v>152</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>152</v>
+        <v>185</v>
       </c>
       <c r="F31" s="7">
         <v>100</v>
@@ -2228,13 +2498,13 @@
         <v>97</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>152</v>
+        <v>215</v>
       </c>
       <c r="K31" s="7" t="s">
         <v>109</v>
       </c>
       <c r="L31" s="4" t="s">
-        <v>152</v>
+        <v>246</v>
       </c>
       <c r="M31" s="7">
         <v>100</v>
@@ -2260,10 +2530,10 @@
         <v>153</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>153</v>
+        <v>186</v>
       </c>
       <c r="F32" s="7">
         <v>100</v>
@@ -2278,13 +2548,13 @@
         <v>97</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>153</v>
+        <v>216</v>
       </c>
       <c r="K32" s="7" t="s">
         <v>109</v>
       </c>
       <c r="L32" s="4" t="s">
-        <v>153</v>
+        <v>247</v>
       </c>
       <c r="M32" s="7">
         <v>100</v>
@@ -2310,10 +2580,10 @@
         <v>154</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>154</v>
+        <v>187</v>
       </c>
       <c r="F33" s="7">
         <v>100</v>
@@ -2328,13 +2598,13 @@
         <v>97</v>
       </c>
       <c r="J33" s="7" t="s">
-        <v>154</v>
+        <v>217</v>
       </c>
       <c r="K33" s="7" t="s">
         <v>109</v>
       </c>
       <c r="L33" s="7" t="s">
-        <v>154</v>
+        <v>248</v>
       </c>
       <c r="M33" s="7">
         <v>100</v>
@@ -2360,10 +2630,10 @@
         <v>155</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>155</v>
+        <v>188</v>
       </c>
       <c r="F34" s="7">
         <v>100</v>
@@ -2378,13 +2648,13 @@
         <v>97</v>
       </c>
       <c r="J34" s="7" t="s">
-        <v>155</v>
+        <v>218</v>
       </c>
       <c r="K34" s="7" t="s">
         <v>109</v>
       </c>
       <c r="L34" s="7" t="s">
-        <v>155</v>
+        <v>249</v>
       </c>
       <c r="M34" s="7">
         <v>100</v>
@@ -2410,10 +2680,10 @@
         <v>156</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>156</v>
+        <v>189</v>
       </c>
       <c r="F35" s="7">
         <v>100</v>
@@ -2428,13 +2698,13 @@
         <v>97</v>
       </c>
       <c r="J35" s="7" t="s">
-        <v>156</v>
+        <v>219</v>
       </c>
       <c r="K35" s="7" t="s">
         <v>109</v>
       </c>
       <c r="L35" s="7" t="s">
-        <v>156</v>
+        <v>250</v>
       </c>
       <c r="M35" s="7">
         <v>100</v>
@@ -2460,10 +2730,10 @@
         <v>157</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>157</v>
+        <v>190</v>
       </c>
       <c r="F37" s="7">
         <v>100</v>
@@ -2478,13 +2748,13 @@
         <v>97</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>157</v>
+        <v>221</v>
       </c>
       <c r="K37" s="7" t="s">
         <v>109</v>
       </c>
       <c r="L37" s="4" t="s">
-        <v>157</v>
+        <v>251</v>
       </c>
       <c r="M37" s="7">
         <v>100</v>
@@ -2510,10 +2780,10 @@
         <v>158</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>158</v>
+        <v>191</v>
       </c>
       <c r="F38" s="7">
         <v>100</v>
@@ -2528,13 +2798,13 @@
         <v>97</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>158</v>
+        <v>220</v>
       </c>
       <c r="K38" s="7" t="s">
         <v>109</v>
       </c>
       <c r="L38" s="4" t="s">
-        <v>158</v>
+        <v>252</v>
       </c>
       <c r="M38" s="7">
         <v>100</v>
@@ -2560,10 +2830,10 @@
         <v>159</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>159</v>
+        <v>192</v>
       </c>
       <c r="F39" s="7">
         <v>100</v>
@@ -2578,13 +2848,13 @@
         <v>97</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>159</v>
+        <v>222</v>
       </c>
       <c r="K39" s="7" t="s">
         <v>109</v>
       </c>
       <c r="L39" s="4" t="s">
-        <v>159</v>
+        <v>253</v>
       </c>
       <c r="M39" s="7">
         <v>100</v>
@@ -2610,10 +2880,10 @@
         <v>160</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>160</v>
+        <v>193</v>
       </c>
       <c r="F40" s="7">
         <v>100</v>
@@ -2628,13 +2898,13 @@
         <v>97</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>160</v>
+        <v>223</v>
       </c>
       <c r="K40" s="7" t="s">
         <v>109</v>
       </c>
       <c r="L40" s="4" t="s">
-        <v>160</v>
+        <v>254</v>
       </c>
       <c r="M40" s="7">
         <v>100</v>
@@ -2660,10 +2930,10 @@
         <v>161</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>161</v>
+        <v>194</v>
       </c>
       <c r="F41" s="7">
         <v>100</v>
@@ -2678,13 +2948,13 @@
         <v>97</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>161</v>
+        <v>224</v>
       </c>
       <c r="K41" s="7" t="s">
         <v>109</v>
       </c>
       <c r="L41" s="4" t="s">
-        <v>161</v>
+        <v>255</v>
       </c>
       <c r="M41" s="7">
         <v>100</v>
@@ -2710,10 +2980,10 @@
         <v>162</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>162</v>
+        <v>195</v>
       </c>
       <c r="F42" s="7">
         <v>100</v>
@@ -2728,13 +2998,13 @@
         <v>97</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>162</v>
+        <v>225</v>
       </c>
       <c r="K42" s="7" t="s">
         <v>109</v>
       </c>
       <c r="L42" s="4" t="s">
-        <v>162</v>
+        <v>256</v>
       </c>
       <c r="M42" s="7">
         <v>100</v>
@@ -2760,10 +3030,10 @@
         <v>163</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>163</v>
+        <v>196</v>
       </c>
       <c r="F43" s="7">
         <v>100</v>
@@ -2778,13 +3048,13 @@
         <v>97</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>163</v>
+        <v>226</v>
       </c>
       <c r="K43" s="7" t="s">
         <v>109</v>
       </c>
       <c r="L43" s="4" t="s">
-        <v>163</v>
+        <v>257</v>
       </c>
       <c r="M43" s="7">
         <v>100</v>
@@ -2810,10 +3080,10 @@
         <v>164</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>164</v>
+        <v>197</v>
       </c>
       <c r="F44" s="7">
         <v>100</v>
@@ -2828,13 +3098,13 @@
         <v>97</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>164</v>
+        <v>227</v>
       </c>
       <c r="K44" s="7" t="s">
         <v>109</v>
       </c>
       <c r="L44" s="4" t="s">
-        <v>164</v>
+        <v>258</v>
       </c>
       <c r="M44" s="7">
         <v>100</v>
@@ -2860,10 +3130,10 @@
         <v>165</v>
       </c>
       <c r="D45" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>165</v>
+        <v>198</v>
       </c>
       <c r="F45" s="7">
         <v>100</v>
@@ -2878,13 +3148,13 @@
         <v>97</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>165</v>
+        <v>228</v>
       </c>
       <c r="K45" s="7" t="s">
         <v>109</v>
       </c>
       <c r="L45" s="4" t="s">
-        <v>165</v>
+        <v>259</v>
       </c>
       <c r="M45" s="7">
         <v>100</v>
@@ -2910,10 +3180,10 @@
         <v>166</v>
       </c>
       <c r="D46" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>166</v>
+        <v>199</v>
       </c>
       <c r="F46" s="7">
         <v>100</v>
@@ -2928,13 +3198,13 @@
         <v>97</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>166</v>
+        <v>229</v>
       </c>
       <c r="K46" s="7" t="s">
         <v>109</v>
       </c>
       <c r="L46" s="4" t="s">
-        <v>166</v>
+        <v>260</v>
       </c>
       <c r="M46" s="7">
         <v>100</v>
@@ -2957,10 +3227,10 @@
         <v>157</v>
       </c>
       <c r="D48" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>157</v>
+        <v>190</v>
       </c>
       <c r="F48" s="7">
         <v>100</v>
@@ -2975,13 +3245,13 @@
         <v>97</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>157</v>
+        <v>221</v>
       </c>
       <c r="K48" s="7" t="s">
         <v>109</v>
       </c>
       <c r="L48" s="4" t="s">
-        <v>157</v>
+        <v>251</v>
       </c>
       <c r="M48" s="7">
         <v>100</v>
@@ -3004,10 +3274,10 @@
         <v>158</v>
       </c>
       <c r="D49" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>158</v>
+        <v>191</v>
       </c>
       <c r="F49" s="7">
         <v>100</v>
@@ -3022,13 +3292,13 @@
         <v>97</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>158</v>
+        <v>220</v>
       </c>
       <c r="K49" s="7" t="s">
         <v>109</v>
       </c>
       <c r="L49" s="4" t="s">
-        <v>158</v>
+        <v>252</v>
       </c>
       <c r="M49" s="7">
         <v>100</v>
@@ -3051,10 +3321,10 @@
         <v>159</v>
       </c>
       <c r="D50" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>159</v>
+        <v>192</v>
       </c>
       <c r="F50" s="7">
         <v>100</v>
@@ -3069,13 +3339,13 @@
         <v>97</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>159</v>
+        <v>222</v>
       </c>
       <c r="K50" s="7" t="s">
         <v>109</v>
       </c>
       <c r="L50" s="4" t="s">
-        <v>159</v>
+        <v>253</v>
       </c>
       <c r="M50" s="7">
         <v>100</v>
@@ -3098,10 +3368,10 @@
         <v>160</v>
       </c>
       <c r="D51" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>160</v>
+        <v>193</v>
       </c>
       <c r="F51" s="7">
         <v>100</v>
@@ -3116,13 +3386,13 @@
         <v>97</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>160</v>
+        <v>223</v>
       </c>
       <c r="K51" s="7" t="s">
         <v>109</v>
       </c>
       <c r="L51" s="4" t="s">
-        <v>160</v>
+        <v>254</v>
       </c>
       <c r="M51" s="7">
         <v>100</v>
@@ -3145,10 +3415,10 @@
         <v>161</v>
       </c>
       <c r="D52" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>161</v>
+        <v>194</v>
       </c>
       <c r="F52" s="7">
         <v>100</v>
@@ -3163,13 +3433,13 @@
         <v>97</v>
       </c>
       <c r="J52" s="4" t="s">
-        <v>161</v>
+        <v>224</v>
       </c>
       <c r="K52" s="7" t="s">
         <v>109</v>
       </c>
       <c r="L52" s="4" t="s">
-        <v>161</v>
+        <v>255</v>
       </c>
       <c r="M52" s="7">
         <v>100</v>
@@ -3192,10 +3462,10 @@
         <v>162</v>
       </c>
       <c r="D53" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>162</v>
+        <v>195</v>
       </c>
       <c r="F53" s="7">
         <v>100</v>
@@ -3210,13 +3480,13 @@
         <v>97</v>
       </c>
       <c r="J53" s="4" t="s">
-        <v>162</v>
+        <v>225</v>
       </c>
       <c r="K53" s="7" t="s">
         <v>109</v>
       </c>
       <c r="L53" s="4" t="s">
-        <v>162</v>
+        <v>256</v>
       </c>
       <c r="M53" s="7">
         <v>100</v>
@@ -3239,10 +3509,10 @@
         <v>163</v>
       </c>
       <c r="D54" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>163</v>
+        <v>196</v>
       </c>
       <c r="F54" s="7">
         <v>100</v>
@@ -3257,13 +3527,13 @@
         <v>97</v>
       </c>
       <c r="J54" s="4" t="s">
-        <v>163</v>
+        <v>226</v>
       </c>
       <c r="K54" s="7" t="s">
         <v>109</v>
       </c>
       <c r="L54" s="4" t="s">
-        <v>163</v>
+        <v>257</v>
       </c>
       <c r="M54" s="7">
         <v>100</v>
@@ -3286,10 +3556,10 @@
         <v>164</v>
       </c>
       <c r="D55" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>164</v>
+        <v>197</v>
       </c>
       <c r="F55" s="7">
         <v>100</v>
@@ -3304,13 +3574,13 @@
         <v>97</v>
       </c>
       <c r="J55" s="4" t="s">
-        <v>164</v>
+        <v>227</v>
       </c>
       <c r="K55" s="7" t="s">
         <v>109</v>
       </c>
       <c r="L55" s="4" t="s">
-        <v>164</v>
+        <v>258</v>
       </c>
       <c r="M55" s="7">
         <v>100</v>
@@ -3333,10 +3603,10 @@
         <v>165</v>
       </c>
       <c r="D56" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>165</v>
+        <v>198</v>
       </c>
       <c r="F56" s="7">
         <v>100</v>
@@ -3351,13 +3621,13 @@
         <v>97</v>
       </c>
       <c r="J56" s="4" t="s">
-        <v>165</v>
+        <v>228</v>
       </c>
       <c r="K56" s="7" t="s">
         <v>109</v>
       </c>
       <c r="L56" s="4" t="s">
-        <v>165</v>
+        <v>259</v>
       </c>
       <c r="M56" s="7">
         <v>100</v>
@@ -3380,10 +3650,10 @@
         <v>166</v>
       </c>
       <c r="D57" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>166</v>
+        <v>199</v>
       </c>
       <c r="F57" s="7">
         <v>100</v>
@@ -3398,13 +3668,13 @@
         <v>97</v>
       </c>
       <c r="J57" s="4" t="s">
-        <v>166</v>
+        <v>229</v>
       </c>
       <c r="K57" s="7" t="s">
         <v>109</v>
       </c>
       <c r="L57" s="4" t="s">
-        <v>166</v>
+        <v>260</v>
       </c>
       <c r="M57" s="7">
         <v>100</v>
@@ -3815,12 +4085,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Generate functional Comet-Farm upload XML
</commit_message>
<xml_diff>
--- a/template_v2.xlsx
+++ b/template_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dpollard/projects/comet/COMET-Farm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC72EA96-E374-4145-9C35-5BF235217FB1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{651DC8DA-8A99-3446-80CF-B805051A33FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="480" windowWidth="32720" windowHeight="20540" xr2:uid="{5384504D-6727-334D-8532-C0C118A2956A}"/>
   </bookViews>
@@ -98,7 +98,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="261">
   <si>
     <t>Yes</t>
   </si>
@@ -1560,8 +1560,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:P57"/>
   <sheetViews>
-    <sheetView showFormulas="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M50" sqref="M50"/>
+    <sheetView showFormulas="1" tabSelected="1" topLeftCell="D39" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N48" sqref="N48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="25" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -3223,6 +3223,9 @@
       <c r="A48" s="4">
         <v>2020</v>
       </c>
+      <c r="B48" s="4" t="s">
+        <v>2</v>
+      </c>
       <c r="C48" s="4" t="s">
         <v>157</v>
       </c>
@@ -3242,7 +3245,7 @@
         <v>0</v>
       </c>
       <c r="I48" s="7" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="J48" s="4" t="s">
         <v>221</v>
@@ -3254,7 +3257,7 @@
         <v>251</v>
       </c>
       <c r="M48" s="7">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="N48" s="7" t="s">
         <v>121</v>
@@ -3270,6 +3273,9 @@
       <c r="A49" s="4">
         <v>2021</v>
       </c>
+      <c r="B49" s="4" t="s">
+        <v>2</v>
+      </c>
       <c r="C49" s="4" t="s">
         <v>158</v>
       </c>
@@ -3289,7 +3295,7 @@
         <v>0</v>
       </c>
       <c r="I49" s="7" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="J49" s="4" t="s">
         <v>220</v>
@@ -3301,7 +3307,7 @@
         <v>252</v>
       </c>
       <c r="M49" s="7">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="N49" s="7" t="s">
         <v>121</v>
@@ -3317,6 +3323,9 @@
       <c r="A50" s="4">
         <v>2022</v>
       </c>
+      <c r="B50" s="4" t="s">
+        <v>2</v>
+      </c>
       <c r="C50" s="4" t="s">
         <v>159</v>
       </c>
@@ -3336,7 +3345,7 @@
         <v>0</v>
       </c>
       <c r="I50" s="7" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="J50" s="4" t="s">
         <v>222</v>
@@ -3348,7 +3357,7 @@
         <v>253</v>
       </c>
       <c r="M50" s="7">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="N50" s="7" t="s">
         <v>121</v>
@@ -3364,6 +3373,9 @@
       <c r="A51" s="4">
         <v>2023</v>
       </c>
+      <c r="B51" s="4" t="s">
+        <v>2</v>
+      </c>
       <c r="C51" s="4" t="s">
         <v>160</v>
       </c>
@@ -3383,7 +3395,7 @@
         <v>0</v>
       </c>
       <c r="I51" s="7" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="J51" s="4" t="s">
         <v>223</v>
@@ -3395,7 +3407,7 @@
         <v>254</v>
       </c>
       <c r="M51" s="7">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="N51" s="7" t="s">
         <v>121</v>
@@ -3411,6 +3423,9 @@
       <c r="A52" s="4">
         <v>2024</v>
       </c>
+      <c r="B52" s="4" t="s">
+        <v>2</v>
+      </c>
       <c r="C52" s="4" t="s">
         <v>161</v>
       </c>
@@ -3430,7 +3445,7 @@
         <v>0</v>
       </c>
       <c r="I52" s="7" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="J52" s="4" t="s">
         <v>224</v>
@@ -3442,7 +3457,7 @@
         <v>255</v>
       </c>
       <c r="M52" s="7">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="N52" s="7" t="s">
         <v>121</v>
@@ -3458,6 +3473,9 @@
       <c r="A53" s="4">
         <v>2025</v>
       </c>
+      <c r="B53" s="4" t="s">
+        <v>2</v>
+      </c>
       <c r="C53" s="4" t="s">
         <v>162</v>
       </c>
@@ -3477,7 +3495,7 @@
         <v>0</v>
       </c>
       <c r="I53" s="7" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="J53" s="4" t="s">
         <v>225</v>
@@ -3489,7 +3507,7 @@
         <v>256</v>
       </c>
       <c r="M53" s="7">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="N53" s="7" t="s">
         <v>121</v>
@@ -3505,6 +3523,9 @@
       <c r="A54" s="4">
         <v>2026</v>
       </c>
+      <c r="B54" s="4" t="s">
+        <v>2</v>
+      </c>
       <c r="C54" s="4" t="s">
         <v>163</v>
       </c>
@@ -3524,7 +3545,7 @@
         <v>0</v>
       </c>
       <c r="I54" s="7" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="J54" s="4" t="s">
         <v>226</v>
@@ -3536,7 +3557,7 @@
         <v>257</v>
       </c>
       <c r="M54" s="7">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="N54" s="7" t="s">
         <v>121</v>
@@ -3552,6 +3573,9 @@
       <c r="A55" s="4">
         <v>2027</v>
       </c>
+      <c r="B55" s="4" t="s">
+        <v>2</v>
+      </c>
       <c r="C55" s="4" t="s">
         <v>164</v>
       </c>
@@ -3571,7 +3595,7 @@
         <v>0</v>
       </c>
       <c r="I55" s="7" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="J55" s="4" t="s">
         <v>227</v>
@@ -3583,7 +3607,7 @@
         <v>258</v>
       </c>
       <c r="M55" s="7">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="N55" s="7" t="s">
         <v>121</v>
@@ -3599,6 +3623,9 @@
       <c r="A56" s="4">
         <v>2028</v>
       </c>
+      <c r="B56" s="4" t="s">
+        <v>2</v>
+      </c>
       <c r="C56" s="4" t="s">
         <v>165</v>
       </c>
@@ -3618,7 +3645,7 @@
         <v>0</v>
       </c>
       <c r="I56" s="7" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="J56" s="4" t="s">
         <v>228</v>
@@ -3630,7 +3657,7 @@
         <v>259</v>
       </c>
       <c r="M56" s="7">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="N56" s="7" t="s">
         <v>121</v>
@@ -3646,6 +3673,9 @@
       <c r="A57" s="4">
         <v>2029</v>
       </c>
+      <c r="B57" s="4" t="s">
+        <v>2</v>
+      </c>
       <c r="C57" s="4" t="s">
         <v>166</v>
       </c>
@@ -3665,7 +3695,7 @@
         <v>0</v>
       </c>
       <c r="I57" s="7" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="J57" s="4" t="s">
         <v>229</v>
@@ -3677,7 +3707,7 @@
         <v>260</v>
       </c>
       <c r="M57" s="7">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="N57" s="7" t="s">
         <v>121</v>

</xml_diff>